<commit_message>
chapter 7 Servlet complete next is jsp
</commit_message>
<xml_diff>
--- a/JSP-SERVLET.xlsx
+++ b/JSP-SERVLET.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet7" sheetId="9" r:id="rId1"/>
+    <sheet name="현황" sheetId="9" r:id="rId1"/>
     <sheet name="Chapter 1" sheetId="1" r:id="rId2"/>
     <sheet name="Chapter 2" sheetId="4" r:id="rId3"/>
     <sheet name="Chapter 3" sheetId="5" r:id="rId4"/>
     <sheet name="Chapter 4" sheetId="6" r:id="rId5"/>
     <sheet name="Chapter 5" sheetId="7" r:id="rId6"/>
     <sheet name="Chapter 6" sheetId="8" r:id="rId7"/>
+    <sheet name="Chapter 7" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t>페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -339,6 +340,15 @@
 4. 세션 개념 이해
 5. 세션 생성 및 상태 확인 실습
 6. HttpServletRequest와 RequestDispatcher를 통한 요구재지정 실습
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고급 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">P.246 ~ P.301
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -611,7 +621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -734,6 +744,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -760,6 +782,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1102,28 +1130,28 @@
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="45"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="52" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="50"/>
+      <c r="D3" s="54"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
@@ -2004,13 +2032,13 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="28"/>
-      <c r="J5" s="64" t="s">
+      <c r="J5" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="71"/>
       <c r="O5" s="27" t="s">
         <v>16</v>
       </c>
@@ -2040,11 +2068,11 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="30"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
       <c r="O6" s="35"/>
       <c r="P6" s="36"/>
       <c r="Q6" s="36"/>
@@ -2068,11 +2096,11 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="30"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="72"/>
       <c r="O7" s="35"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
@@ -2096,11 +2124,11 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="30"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="72"/>
       <c r="O8" s="35"/>
       <c r="P8" s="36"/>
       <c r="Q8" s="36"/>
@@ -2124,11 +2152,11 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="30"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="66"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="72"/>
       <c r="O9" s="35"/>
       <c r="P9" s="36"/>
       <c r="Q9" s="36"/>
@@ -2152,11 +2180,11 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="30"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
       <c r="O10" s="35"/>
       <c r="P10" s="36"/>
       <c r="Q10" s="36"/>
@@ -2180,11 +2208,11 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="72"/>
       <c r="O11" s="35"/>
       <c r="P11" s="36"/>
       <c r="Q11" s="36"/>
@@ -2208,11 +2236,11 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="30"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="72"/>
       <c r="O12" s="35"/>
       <c r="P12" s="36"/>
       <c r="Q12" s="36"/>
@@ -2236,11 +2264,11 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="30"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="66"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="72"/>
       <c r="O13" s="35"/>
       <c r="P13" s="36"/>
       <c r="Q13" s="36"/>
@@ -2264,11 +2292,11 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="30"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="66"/>
-      <c r="N14" s="66"/>
+      <c r="J14" s="72"/>
+      <c r="K14" s="72"/>
+      <c r="L14" s="72"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="72"/>
       <c r="O14" s="35"/>
       <c r="P14" s="36"/>
       <c r="Q14" s="36"/>
@@ -2292,11 +2320,11 @@
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
       <c r="I15" s="33"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="67"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
       <c r="O15" s="38"/>
       <c r="P15" s="39"/>
       <c r="Q15" s="39"/>
@@ -2566,13 +2594,13 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="28"/>
-      <c r="J5" s="64" t="s">
+      <c r="J5" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="71"/>
       <c r="O5" s="27" t="s">
         <v>21</v>
       </c>
@@ -2602,11 +2630,11 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="30"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
       <c r="O6" s="35"/>
       <c r="P6" s="36"/>
       <c r="Q6" s="36"/>
@@ -2630,11 +2658,11 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="30"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="72"/>
       <c r="O7" s="35"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
@@ -2658,11 +2686,11 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="30"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="72"/>
       <c r="O8" s="35"/>
       <c r="P8" s="36"/>
       <c r="Q8" s="36"/>
@@ -2686,11 +2714,11 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="30"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="66"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="72"/>
       <c r="O9" s="35"/>
       <c r="P9" s="36"/>
       <c r="Q9" s="36"/>
@@ -2714,11 +2742,11 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="30"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
       <c r="O10" s="35"/>
       <c r="P10" s="36"/>
       <c r="Q10" s="36"/>
@@ -2742,11 +2770,11 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="72"/>
       <c r="O11" s="35"/>
       <c r="P11" s="36"/>
       <c r="Q11" s="36"/>
@@ -2770,11 +2798,11 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="30"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="72"/>
       <c r="O12" s="35"/>
       <c r="P12" s="36"/>
       <c r="Q12" s="36"/>
@@ -2798,11 +2826,11 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="30"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="66"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="72"/>
+      <c r="M13" s="72"/>
+      <c r="N13" s="72"/>
       <c r="O13" s="35"/>
       <c r="P13" s="36"/>
       <c r="Q13" s="36"/>
@@ -2826,11 +2854,11 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="30"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="66"/>
-      <c r="N14" s="66"/>
+      <c r="J14" s="72"/>
+      <c r="K14" s="72"/>
+      <c r="L14" s="72"/>
+      <c r="M14" s="72"/>
+      <c r="N14" s="72"/>
       <c r="O14" s="35"/>
       <c r="P14" s="36"/>
       <c r="Q14" s="36"/>
@@ -2854,11 +2882,11 @@
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
       <c r="I15" s="33"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="67"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
       <c r="O15" s="38"/>
       <c r="P15" s="39"/>
       <c r="Q15" s="39"/>
@@ -3128,10 +3156,10 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="28"/>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="59"/>
+      <c r="K5" s="65"/>
       <c r="L5" s="27" t="s">
         <v>24</v>
       </c>
@@ -3146,7 +3174,7 @@
       <c r="S5" s="18"/>
       <c r="T5" s="18"/>
       <c r="U5" s="18"/>
-      <c r="V5" s="51"/>
+      <c r="V5" s="57"/>
       <c r="W5" s="41" t="s">
         <v>8</v>
       </c>
@@ -3164,19 +3192,19 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="30"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="61"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="67"/>
       <c r="L6" s="29"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="30"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="54"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="60"/>
       <c r="W6" s="10"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
@@ -3192,19 +3220,19 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="30"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="61"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="67"/>
       <c r="L7" s="29"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="30"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="54"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="59"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="59"/>
+      <c r="V7" s="60"/>
       <c r="W7" s="10"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
@@ -3220,19 +3248,19 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="30"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="61"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="67"/>
       <c r="L8" s="29"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="30"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="53"/>
-      <c r="T8" s="53"/>
-      <c r="U8" s="53"/>
-      <c r="V8" s="54"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="59"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
+      <c r="U8" s="59"/>
+      <c r="V8" s="60"/>
       <c r="W8" s="10"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
@@ -3248,19 +3276,19 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="30"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="67"/>
       <c r="L9" s="29"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="30"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="53"/>
-      <c r="S9" s="53"/>
-      <c r="T9" s="53"/>
-      <c r="U9" s="53"/>
-      <c r="V9" s="54"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="59"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="59"/>
+      <c r="U9" s="59"/>
+      <c r="V9" s="60"/>
       <c r="W9" s="10"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
@@ -3276,19 +3304,19 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="30"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="63"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="69"/>
       <c r="L10" s="29"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="30"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="53"/>
-      <c r="S10" s="53"/>
-      <c r="T10" s="53"/>
-      <c r="U10" s="53"/>
-      <c r="V10" s="54"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="59"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
+      <c r="U10" s="59"/>
+      <c r="V10" s="60"/>
       <c r="W10" s="10"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -3304,21 +3332,21 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="59"/>
+      <c r="K11" s="65"/>
       <c r="L11" s="29"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="30"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="53"/>
-      <c r="S11" s="53"/>
-      <c r="T11" s="53"/>
-      <c r="U11" s="53"/>
-      <c r="V11" s="54"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
+      <c r="U11" s="59"/>
+      <c r="V11" s="60"/>
       <c r="W11" s="10"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -3334,19 +3362,19 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="30"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="61"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="67"/>
       <c r="L12" s="29"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="30"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="53"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="53"/>
-      <c r="V12" s="54"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="59"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="59"/>
+      <c r="U12" s="59"/>
+      <c r="V12" s="60"/>
       <c r="W12" s="10"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -3362,19 +3390,19 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="30"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="61"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="67"/>
       <c r="L13" s="29"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="30"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="53"/>
-      <c r="S13" s="53"/>
-      <c r="T13" s="53"/>
-      <c r="U13" s="53"/>
-      <c r="V13" s="54"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="59"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
+      <c r="U13" s="59"/>
+      <c r="V13" s="60"/>
       <c r="W13" s="10"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
@@ -3390,19 +3418,19 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="30"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="61"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="67"/>
       <c r="L14" s="29"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="30"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="53"/>
-      <c r="S14" s="53"/>
-      <c r="T14" s="53"/>
-      <c r="U14" s="53"/>
-      <c r="V14" s="54"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="59"/>
+      <c r="S14" s="59"/>
+      <c r="T14" s="59"/>
+      <c r="U14" s="59"/>
+      <c r="V14" s="60"/>
       <c r="W14" s="10"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
@@ -3418,19 +3446,19 @@
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
       <c r="I15" s="33"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="63"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="69"/>
       <c r="L15" s="31"/>
       <c r="M15" s="32"/>
       <c r="N15" s="32"/>
       <c r="O15" s="32"/>
       <c r="P15" s="33"/>
-      <c r="Q15" s="55"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="56"/>
-      <c r="U15" s="56"/>
-      <c r="V15" s="57"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="62"/>
+      <c r="V15" s="63"/>
       <c r="W15" s="12"/>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
@@ -3692,10 +3720,10 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="28"/>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="59"/>
+      <c r="K5" s="65"/>
       <c r="L5" s="27" t="s">
         <v>32</v>
       </c>
@@ -3728,8 +3756,8 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="30"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="61"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="67"/>
       <c r="L6" s="29"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -3756,8 +3784,8 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="30"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="61"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="67"/>
       <c r="L7" s="29"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -3784,8 +3812,8 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="30"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="61"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="67"/>
       <c r="L8" s="29"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -3812,8 +3840,8 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="30"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="67"/>
       <c r="L9" s="29"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -3840,8 +3868,8 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="30"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="63"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="69"/>
       <c r="L10" s="29"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -3868,10 +3896,10 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="K11" s="59"/>
+      <c r="K11" s="65"/>
       <c r="L11" s="29"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
@@ -3898,8 +3926,8 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="30"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="61"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="67"/>
       <c r="L12" s="29"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -3926,8 +3954,8 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="30"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="61"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="67"/>
       <c r="L13" s="29"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
@@ -3954,8 +3982,8 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="30"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="61"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="67"/>
       <c r="L14" s="29"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -3982,8 +4010,8 @@
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
       <c r="I15" s="33"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="63"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="69"/>
       <c r="L15" s="31"/>
       <c r="M15" s="32"/>
       <c r="N15" s="32"/>
@@ -4111,7 +4139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
@@ -4257,10 +4285,10 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="28"/>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="59"/>
+      <c r="K5" s="65"/>
       <c r="L5" s="27" t="s">
         <v>61</v>
       </c>
@@ -4275,7 +4303,7 @@
       <c r="S5" s="18"/>
       <c r="T5" s="18"/>
       <c r="U5" s="18"/>
-      <c r="V5" s="51"/>
+      <c r="V5" s="57"/>
       <c r="W5" s="41" t="s">
         <v>8</v>
       </c>
@@ -4293,19 +4321,19 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="30"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="61"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="67"/>
       <c r="L6" s="29"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
-      <c r="V6" s="54"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="60"/>
       <c r="W6" s="10"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
@@ -4321,19 +4349,19 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="30"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="61"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="67"/>
       <c r="L7" s="29"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="53"/>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
-      <c r="V7" s="54"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="59"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="59"/>
+      <c r="V7" s="60"/>
       <c r="W7" s="10"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
@@ -4349,19 +4377,19 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="30"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="61"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="67"/>
       <c r="L8" s="29"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="53"/>
-      <c r="T8" s="53"/>
-      <c r="U8" s="53"/>
-      <c r="V8" s="54"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="59"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
+      <c r="U8" s="59"/>
+      <c r="V8" s="60"/>
       <c r="W8" s="10"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
@@ -4377,19 +4405,19 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="30"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="67"/>
       <c r="L9" s="29"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="53"/>
-      <c r="S9" s="53"/>
-      <c r="T9" s="53"/>
-      <c r="U9" s="53"/>
-      <c r="V9" s="54"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="59"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="59"/>
+      <c r="U9" s="59"/>
+      <c r="V9" s="60"/>
       <c r="W9" s="10"/>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
@@ -4405,19 +4433,19 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="30"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="63"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="69"/>
       <c r="L10" s="29"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="53"/>
-      <c r="S10" s="53"/>
-      <c r="T10" s="53"/>
-      <c r="U10" s="53"/>
-      <c r="V10" s="54"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="59"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
+      <c r="U10" s="59"/>
+      <c r="V10" s="60"/>
       <c r="W10" s="10"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
@@ -4433,21 +4461,21 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="59"/>
+      <c r="K11" s="65"/>
       <c r="L11" s="29"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="53"/>
-      <c r="S11" s="53"/>
-      <c r="T11" s="53"/>
-      <c r="U11" s="53"/>
-      <c r="V11" s="54"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
+      <c r="U11" s="59"/>
+      <c r="V11" s="60"/>
       <c r="W11" s="10"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -4463,19 +4491,19 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="30"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="61"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="67"/>
       <c r="L12" s="29"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="53"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="53"/>
-      <c r="V12" s="54"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="59"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="59"/>
+      <c r="U12" s="59"/>
+      <c r="V12" s="60"/>
       <c r="W12" s="10"/>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
@@ -4491,19 +4519,19 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="30"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="61"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="67"/>
       <c r="L13" s="29"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="53"/>
-      <c r="S13" s="53"/>
-      <c r="T13" s="53"/>
-      <c r="U13" s="53"/>
-      <c r="V13" s="54"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="59"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
+      <c r="U13" s="59"/>
+      <c r="V13" s="60"/>
       <c r="W13" s="10"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
@@ -4519,19 +4547,19 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="30"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="61"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="67"/>
       <c r="L14" s="29"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="53"/>
-      <c r="S14" s="53"/>
-      <c r="T14" s="53"/>
-      <c r="U14" s="53"/>
-      <c r="V14" s="54"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="59"/>
+      <c r="S14" s="59"/>
+      <c r="T14" s="59"/>
+      <c r="U14" s="59"/>
+      <c r="V14" s="60"/>
       <c r="W14" s="10"/>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
@@ -4547,19 +4575,19 @@
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
       <c r="I15" s="33"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="63"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="69"/>
       <c r="L15" s="31"/>
       <c r="M15" s="32"/>
       <c r="N15" s="32"/>
       <c r="O15" s="32"/>
       <c r="P15" s="32"/>
-      <c r="Q15" s="55"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="56"/>
-      <c r="U15" s="56"/>
-      <c r="V15" s="57"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="62"/>
+      <c r="V15" s="63"/>
       <c r="W15" s="12"/>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
@@ -4670,4 +4698,565 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5:V15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="9"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A2" s="10"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="11"/>
+    </row>
+    <row r="3" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="14"/>
+    </row>
+    <row r="4" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="16"/>
+      <c r="L4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="14"/>
+    </row>
+    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="65"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="57"/>
+      <c r="W5" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="9"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="60"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="11"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="59"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="59"/>
+      <c r="V7" s="60"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="11"/>
+    </row>
+    <row r="8" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="59"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
+      <c r="U8" s="59"/>
+      <c r="V8" s="60"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="11"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="59"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="59"/>
+      <c r="U9" s="59"/>
+      <c r="V9" s="60"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="11"/>
+    </row>
+    <row r="10" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="59"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
+      <c r="U10" s="59"/>
+      <c r="V10" s="60"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="11"/>
+    </row>
+    <row r="11" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="43"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
+      <c r="U11" s="59"/>
+      <c r="V11" s="60"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="11"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="59"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="59"/>
+      <c r="U12" s="59"/>
+      <c r="V12" s="60"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="11"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="59"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
+      <c r="U13" s="59"/>
+      <c r="V13" s="60"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="11"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="59"/>
+      <c r="S14" s="59"/>
+      <c r="T14" s="59"/>
+      <c r="U14" s="59"/>
+      <c r="V14" s="60"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="11"/>
+    </row>
+    <row r="15" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="62"/>
+      <c r="V15" s="63"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="14"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="C5:I15"/>
+    <mergeCell ref="J5:K10"/>
+    <mergeCell ref="L5:P15"/>
+    <mergeCell ref="Q5:V15"/>
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="J11:K15"/>
+    <mergeCell ref="A1:Z3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="W4:Z4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J11:K15" r:id="rId1" display="https://github.com/phc09188/JSP-Study/tree/main/src/main/java/com/example/jsptest/chapter7"/>
+    <hyperlink ref="J5:K10" r:id="rId2" display="https://github.com/phc09188/JSP-Study/tree/main/src/main/webapp"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chapter 12 EL commit
</commit_message>
<xml_diff>
--- a/JSP-SERVLET.xlsx
+++ b/JSP-SERVLET.xlsx
@@ -9,20 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="현황" sheetId="9" r:id="rId1"/>
     <sheet name="Chapter 1" sheetId="1" r:id="rId2"/>
-    <sheet name="Chapter 2" sheetId="4" r:id="rId3"/>
-    <sheet name="Chapter 3" sheetId="5" r:id="rId4"/>
-    <sheet name="Chapter 4" sheetId="6" r:id="rId5"/>
-    <sheet name="Chapter 5" sheetId="7" r:id="rId6"/>
-    <sheet name="Chapter 6" sheetId="8" r:id="rId7"/>
-    <sheet name="Chapter 7" sheetId="10" r:id="rId8"/>
-    <sheet name="Chapter 8" sheetId="11" r:id="rId9"/>
-    <sheet name="Chapter 9" sheetId="12" r:id="rId10"/>
-    <sheet name="Chapter 10" sheetId="13" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId3"/>
+    <sheet name="Chapter 2" sheetId="4" r:id="rId4"/>
+    <sheet name="Chapter 3" sheetId="5" r:id="rId5"/>
+    <sheet name="Chapter 4" sheetId="6" r:id="rId6"/>
+    <sheet name="Chapter 5" sheetId="7" r:id="rId7"/>
+    <sheet name="Chapter 6" sheetId="8" r:id="rId8"/>
+    <sheet name="Chapter 7" sheetId="10" r:id="rId9"/>
+    <sheet name="Chapter 8" sheetId="11" r:id="rId10"/>
+    <sheet name="Chapter 9" sheetId="12" r:id="rId11"/>
+    <sheet name="Chapter 10" sheetId="13" r:id="rId12"/>
+    <sheet name="Chapter 11" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="91">
   <si>
     <t>페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -465,6 +467,62 @@
   </si>
   <si>
     <t xml:space="preserve">P.358 ~ P.377
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 표준액션태그란?
+2. 표준액션태그 종류 및 개념
+3. JSP 자바빈즈란?
+4. JSP 자바빈즈 개발 규약
+5. 자바빈즈 실습
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">JSP
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Bean파일
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 자바빈즈를 사용하기 위한 빈즈 객체 생성
+2. JSP를 통해 자바빈즈 사용
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터베이스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">P.381 ~ P.414
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. DB 설치 ( 책 = 오라클, 진행 = mysql로 설치했습니다.)
+2.JDBC 개념 및 동작과정
+3. JSP에서 JDBC를 통해 접근하는 방법
+4. DataSource 객체를 이용한 프로젝트 설정
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. MySQL 환경 설치
+2. JDBC를 통해 jsp와 DB 통신 및 간단한 CRU 작업
+3. datasource 생성을 위한 server.xml, web.xml, context.html 수정
+4. datasource를 통해 JSP와 DB 통신
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">JSP
+dataSource,jdbc.jsp
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -896,6 +954,24 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -920,28 +996,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
@@ -955,27 +1034,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1465,25 +1523,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C17:D17"/>
@@ -1498,6 +1537,25 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1508,15 +1566,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22:L23"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5:Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -1642,11 +1700,11 @@
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="33" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
@@ -1655,24 +1713,24 @@
       <c r="H5" s="34"/>
       <c r="I5" s="35"/>
       <c r="J5" s="68" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5" s="69"/>
+        <v>73</v>
+      </c>
+      <c r="K5" s="76"/>
       <c r="L5" s="33" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="M5" s="34"/>
       <c r="N5" s="34"/>
       <c r="O5" s="34"/>
       <c r="P5" s="34"/>
-      <c r="Q5" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
-      <c r="V5" s="55"/>
+      <c r="Q5" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="35"/>
       <c r="W5" s="31" t="s">
         <v>7</v>
       </c>
@@ -1690,19 +1748,19 @@
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
       <c r="I6" s="38"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="78"/>
       <c r="L6" s="36"/>
       <c r="M6" s="37"/>
       <c r="N6" s="37"/>
       <c r="O6" s="37"/>
       <c r="P6" s="37"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="57"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="57"/>
-      <c r="U6" s="57"/>
-      <c r="V6" s="58"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="38"/>
       <c r="W6" s="17"/>
       <c r="X6" s="18"/>
       <c r="Y6" s="18"/>
@@ -1718,19 +1776,19 @@
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
       <c r="I7" s="38"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="71"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="78"/>
       <c r="L7" s="36"/>
       <c r="M7" s="37"/>
       <c r="N7" s="37"/>
       <c r="O7" s="37"/>
       <c r="P7" s="37"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="57"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="57"/>
-      <c r="V7" s="58"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="38"/>
       <c r="W7" s="17"/>
       <c r="X7" s="18"/>
       <c r="Y7" s="18"/>
@@ -1746,19 +1804,19 @@
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
       <c r="I8" s="38"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="71"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="78"/>
       <c r="L8" s="36"/>
       <c r="M8" s="37"/>
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
       <c r="P8" s="37"/>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="57"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="57"/>
-      <c r="U8" s="57"/>
-      <c r="V8" s="58"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="38"/>
       <c r="W8" s="17"/>
       <c r="X8" s="18"/>
       <c r="Y8" s="18"/>
@@ -1774,19 +1832,19 @@
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
       <c r="I9" s="38"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="71"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="78"/>
       <c r="L9" s="36"/>
       <c r="M9" s="37"/>
       <c r="N9" s="37"/>
       <c r="O9" s="37"/>
       <c r="P9" s="37"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
-      <c r="U9" s="57"/>
-      <c r="V9" s="58"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="38"/>
       <c r="W9" s="17"/>
       <c r="X9" s="18"/>
       <c r="Y9" s="18"/>
@@ -1802,19 +1860,19 @@
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
       <c r="I10" s="38"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="71"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="78"/>
       <c r="L10" s="36"/>
       <c r="M10" s="37"/>
       <c r="N10" s="37"/>
       <c r="O10" s="37"/>
       <c r="P10" s="37"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="57"/>
-      <c r="T10" s="57"/>
-      <c r="U10" s="57"/>
-      <c r="V10" s="58"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="37"/>
+      <c r="U10" s="37"/>
+      <c r="V10" s="38"/>
       <c r="W10" s="17"/>
       <c r="X10" s="18"/>
       <c r="Y10" s="18"/>
@@ -1830,19 +1888,19 @@
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
       <c r="I11" s="38"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="71"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="78"/>
       <c r="L11" s="36"/>
       <c r="M11" s="37"/>
       <c r="N11" s="37"/>
       <c r="O11" s="37"/>
       <c r="P11" s="37"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="57"/>
-      <c r="U11" s="57"/>
-      <c r="V11" s="58"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="37"/>
+      <c r="V11" s="38"/>
       <c r="W11" s="17"/>
       <c r="X11" s="18"/>
       <c r="Y11" s="18"/>
@@ -1858,19 +1916,19 @@
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="38"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="71"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="78"/>
       <c r="L12" s="36"/>
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
       <c r="O12" s="37"/>
       <c r="P12" s="37"/>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="57"/>
-      <c r="U12" s="57"/>
-      <c r="V12" s="58"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="38"/>
       <c r="W12" s="17"/>
       <c r="X12" s="18"/>
       <c r="Y12" s="18"/>
@@ -1886,19 +1944,19 @@
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="38"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="71"/>
+      <c r="J13" s="77"/>
+      <c r="K13" s="78"/>
       <c r="L13" s="36"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
       <c r="O13" s="37"/>
       <c r="P13" s="37"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="57"/>
-      <c r="V13" s="58"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="38"/>
       <c r="W13" s="17"/>
       <c r="X13" s="18"/>
       <c r="Y13" s="18"/>
@@ -1914,19 +1972,19 @@
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="71"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="78"/>
       <c r="L14" s="36"/>
       <c r="M14" s="37"/>
       <c r="N14" s="37"/>
       <c r="O14" s="37"/>
       <c r="P14" s="37"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="58"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="38"/>
       <c r="W14" s="17"/>
       <c r="X14" s="18"/>
       <c r="Y14" s="18"/>
@@ -1942,19 +2000,19 @@
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" s="41"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="73"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="80"/>
       <c r="L15" s="39"/>
       <c r="M15" s="40"/>
       <c r="N15" s="40"/>
       <c r="O15" s="40"/>
       <c r="P15" s="40"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-      <c r="U15" s="60"/>
-      <c r="V15" s="61"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="41"/>
       <c r="W15" s="20"/>
       <c r="X15" s="21"/>
       <c r="Y15" s="21"/>
@@ -2042,12 +2100,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A5:B15"/>
-    <mergeCell ref="C5:I15"/>
-    <mergeCell ref="J5:K15"/>
-    <mergeCell ref="L5:P15"/>
-    <mergeCell ref="Q5:V15"/>
-    <mergeCell ref="W5:Z15"/>
     <mergeCell ref="A1:Z3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:I4"/>
@@ -2055,6 +2107,12 @@
     <mergeCell ref="L4:P4"/>
     <mergeCell ref="Q4:V4"/>
     <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="C5:I15"/>
+    <mergeCell ref="L5:P15"/>
+    <mergeCell ref="Q5:V15"/>
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="J5:K15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2062,6 +2120,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2070,14 +2129,14 @@
   <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:I15"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -2203,10 +2262,12 @@
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B5" s="26"/>
-      <c r="C5" s="33"/>
+      <c r="C5" s="33" t="s">
+        <v>77</v>
+      </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
       <c r="F5" s="34"/>
@@ -2216,8 +2277,10 @@
       <c r="J5" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="69"/>
-      <c r="L5" s="33"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="33" t="s">
+        <v>79</v>
+      </c>
       <c r="M5" s="34"/>
       <c r="N5" s="34"/>
       <c r="O5" s="34"/>
@@ -2225,11 +2288,11 @@
       <c r="Q5" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
-      <c r="V5" s="55"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="61"/>
       <c r="W5" s="31" t="s">
         <v>7</v>
       </c>
@@ -2247,19 +2310,19 @@
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
       <c r="I6" s="38"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="78"/>
       <c r="L6" s="36"/>
       <c r="M6" s="37"/>
       <c r="N6" s="37"/>
       <c r="O6" s="37"/>
       <c r="P6" s="37"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="57"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="57"/>
-      <c r="U6" s="57"/>
-      <c r="V6" s="58"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="64"/>
       <c r="W6" s="17"/>
       <c r="X6" s="18"/>
       <c r="Y6" s="18"/>
@@ -2275,19 +2338,19 @@
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
       <c r="I7" s="38"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="71"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="78"/>
       <c r="L7" s="36"/>
       <c r="M7" s="37"/>
       <c r="N7" s="37"/>
       <c r="O7" s="37"/>
       <c r="P7" s="37"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="57"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="57"/>
-      <c r="V7" s="58"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="64"/>
       <c r="W7" s="17"/>
       <c r="X7" s="18"/>
       <c r="Y7" s="18"/>
@@ -2303,19 +2366,19 @@
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
       <c r="I8" s="38"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="71"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="78"/>
       <c r="L8" s="36"/>
       <c r="M8" s="37"/>
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
       <c r="P8" s="37"/>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="57"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="57"/>
-      <c r="U8" s="57"/>
-      <c r="V8" s="58"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="64"/>
       <c r="W8" s="17"/>
       <c r="X8" s="18"/>
       <c r="Y8" s="18"/>
@@ -2331,19 +2394,19 @@
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
       <c r="I9" s="38"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="71"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="78"/>
       <c r="L9" s="36"/>
       <c r="M9" s="37"/>
       <c r="N9" s="37"/>
       <c r="O9" s="37"/>
       <c r="P9" s="37"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
-      <c r="U9" s="57"/>
-      <c r="V9" s="58"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="64"/>
       <c r="W9" s="17"/>
       <c r="X9" s="18"/>
       <c r="Y9" s="18"/>
@@ -2359,19 +2422,19 @@
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
       <c r="I10" s="38"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="71"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="78"/>
       <c r="L10" s="36"/>
       <c r="M10" s="37"/>
       <c r="N10" s="37"/>
       <c r="O10" s="37"/>
       <c r="P10" s="37"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="57"/>
-      <c r="T10" s="57"/>
-      <c r="U10" s="57"/>
-      <c r="V10" s="58"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="64"/>
       <c r="W10" s="17"/>
       <c r="X10" s="18"/>
       <c r="Y10" s="18"/>
@@ -2387,19 +2450,19 @@
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
       <c r="I11" s="38"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="71"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="78"/>
       <c r="L11" s="36"/>
       <c r="M11" s="37"/>
       <c r="N11" s="37"/>
       <c r="O11" s="37"/>
       <c r="P11" s="37"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="57"/>
-      <c r="U11" s="57"/>
-      <c r="V11" s="58"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="64"/>
       <c r="W11" s="17"/>
       <c r="X11" s="18"/>
       <c r="Y11" s="18"/>
@@ -2415,19 +2478,19 @@
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="38"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="71"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="78"/>
       <c r="L12" s="36"/>
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
       <c r="O12" s="37"/>
       <c r="P12" s="37"/>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="57"/>
-      <c r="U12" s="57"/>
-      <c r="V12" s="58"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="64"/>
       <c r="W12" s="17"/>
       <c r="X12" s="18"/>
       <c r="Y12" s="18"/>
@@ -2443,19 +2506,19 @@
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="38"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="71"/>
+      <c r="J13" s="77"/>
+      <c r="K13" s="78"/>
       <c r="L13" s="36"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
       <c r="O13" s="37"/>
       <c r="P13" s="37"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="57"/>
-      <c r="V13" s="58"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="64"/>
       <c r="W13" s="17"/>
       <c r="X13" s="18"/>
       <c r="Y13" s="18"/>
@@ -2471,19 +2534,19 @@
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="71"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="78"/>
       <c r="L14" s="36"/>
       <c r="M14" s="37"/>
       <c r="N14" s="37"/>
       <c r="O14" s="37"/>
       <c r="P14" s="37"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="58"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="64"/>
       <c r="W14" s="17"/>
       <c r="X14" s="18"/>
       <c r="Y14" s="18"/>
@@ -2499,19 +2562,19 @@
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" s="41"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="73"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="80"/>
       <c r="L15" s="39"/>
       <c r="M15" s="40"/>
       <c r="N15" s="40"/>
       <c r="O15" s="40"/>
       <c r="P15" s="40"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-      <c r="U15" s="60"/>
-      <c r="V15" s="61"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="67"/>
       <c r="W15" s="20"/>
       <c r="X15" s="21"/>
       <c r="Y15" s="21"/>
@@ -2599,11 +2662,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A5:B15"/>
-    <mergeCell ref="C5:I15"/>
-    <mergeCell ref="J5:K15"/>
-    <mergeCell ref="L5:P15"/>
-    <mergeCell ref="Q5:V15"/>
     <mergeCell ref="W5:Z15"/>
     <mergeCell ref="A1:Z3"/>
     <mergeCell ref="A4:B4"/>
@@ -2612,6 +2670,11 @@
     <mergeCell ref="L4:P4"/>
     <mergeCell ref="Q4:V4"/>
     <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="C5:I15"/>
+    <mergeCell ref="J5:K15"/>
+    <mergeCell ref="L5:P15"/>
+    <mergeCell ref="Q5:V15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2622,19 +2685,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5:V15"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -2733,6 +2796,1132 @@
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
       <c r="J4" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="24"/>
+      <c r="L4" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="22"/>
+    </row>
+    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="75"/>
+      <c r="L5" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="61"/>
+      <c r="W5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="12"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="19"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="64"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="19"/>
+    </row>
+    <row r="8" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="64"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="19"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="19"/>
+    </row>
+    <row r="10" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="64"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="19"/>
+    </row>
+    <row r="11" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="69"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="19"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="64"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="19"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A13" s="27"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="64"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="19"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="64"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="19"/>
+    </row>
+    <row r="15" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="67"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
+      <c r="Z15" s="22"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="A1:Z3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="J5:K10"/>
+    <mergeCell ref="J11:K15"/>
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="C5:I15"/>
+    <mergeCell ref="L5:P15"/>
+    <mergeCell ref="Q5:V15"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J11:K15" r:id="rId1" display="https://github.com/phc09188/JSP-Study/blob/main/src/main/java/com/example/jsptest/chapter10/beans/HelloBean.java"/>
+    <hyperlink ref="J5:K10" r:id="rId2" display="https://github.com/phc09188/JSP-Study/blob/main/src/main/webapp/been.jsp"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="12"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="19"/>
+    </row>
+    <row r="3" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="22"/>
+    </row>
+    <row r="4" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="24"/>
+      <c r="L4" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="22"/>
+    </row>
+    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" s="76"/>
+      <c r="L5" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="61"/>
+      <c r="W5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="12"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="19"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="64"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="19"/>
+    </row>
+    <row r="8" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="64"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="19"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="19"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="64"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="19"/>
+    </row>
+    <row r="11" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="19"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="64"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="19"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A13" s="27"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="77"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="64"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="19"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="64"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="19"/>
+    </row>
+    <row r="15" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="67"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
+      <c r="Z15" s="22"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="C5:I15"/>
+    <mergeCell ref="L5:P15"/>
+    <mergeCell ref="Q5:V15"/>
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="J5:K15"/>
+    <mergeCell ref="A1:Z3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="W4:Z4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J5:K15" r:id="rId1" display="https://github.com/phc09188/JSP-Study/tree/main/src/main/webapp"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z35"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="12"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="19"/>
+    </row>
+    <row r="3" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="22"/>
+    </row>
+    <row r="4" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="23" t="s">
         <v>13</v>
       </c>
       <c r="K4" s="32"/>
@@ -3182,6 +4371,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -3718,6 +4921,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="O5:R15"/>
+    <mergeCell ref="S5:V15"/>
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="J5:N15"/>
+    <mergeCell ref="C5:I15"/>
     <mergeCell ref="A1:Z3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="O4:R4"/>
@@ -3725,12 +4934,6 @@
     <mergeCell ref="W4:Z4"/>
     <mergeCell ref="J4:N4"/>
     <mergeCell ref="C4:I4"/>
-    <mergeCell ref="A5:B15"/>
-    <mergeCell ref="O5:R15"/>
-    <mergeCell ref="S5:V15"/>
-    <mergeCell ref="W5:Z15"/>
-    <mergeCell ref="J5:N15"/>
-    <mergeCell ref="C5:I15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3742,7 +4945,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z35"/>
   <sheetViews>
@@ -4304,7 +5507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z35"/>
   <sheetViews>
@@ -4454,10 +5657,10 @@
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
       <c r="I5" s="35"/>
-      <c r="J5" s="62" t="s">
+      <c r="J5" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="63"/>
+      <c r="K5" s="55"/>
       <c r="L5" s="33" t="s">
         <v>24</v>
       </c>
@@ -4468,11 +5671,11 @@
       <c r="Q5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
-      <c r="V5" s="55"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="61"/>
       <c r="W5" s="31" t="s">
         <v>8</v>
       </c>
@@ -4490,19 +5693,19 @@
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
       <c r="I6" s="38"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="65"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
       <c r="L6" s="36"/>
       <c r="M6" s="37"/>
       <c r="N6" s="37"/>
       <c r="O6" s="37"/>
       <c r="P6" s="38"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="57"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="57"/>
-      <c r="U6" s="57"/>
-      <c r="V6" s="58"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="64"/>
       <c r="W6" s="17"/>
       <c r="X6" s="18"/>
       <c r="Y6" s="18"/>
@@ -4518,19 +5721,19 @@
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
       <c r="I7" s="38"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="65"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="36"/>
       <c r="M7" s="37"/>
       <c r="N7" s="37"/>
       <c r="O7" s="37"/>
       <c r="P7" s="38"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="57"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="57"/>
-      <c r="V7" s="58"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="64"/>
       <c r="W7" s="17"/>
       <c r="X7" s="18"/>
       <c r="Y7" s="18"/>
@@ -4546,19 +5749,19 @@
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
       <c r="I8" s="38"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="65"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
       <c r="L8" s="36"/>
       <c r="M8" s="37"/>
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
       <c r="P8" s="38"/>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="57"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="57"/>
-      <c r="U8" s="57"/>
-      <c r="V8" s="58"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="64"/>
       <c r="W8" s="17"/>
       <c r="X8" s="18"/>
       <c r="Y8" s="18"/>
@@ -4574,19 +5777,19 @@
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
       <c r="I9" s="38"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="65"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="36"/>
       <c r="M9" s="37"/>
       <c r="N9" s="37"/>
       <c r="O9" s="37"/>
       <c r="P9" s="38"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
-      <c r="U9" s="57"/>
-      <c r="V9" s="58"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="64"/>
       <c r="W9" s="17"/>
       <c r="X9" s="18"/>
       <c r="Y9" s="18"/>
@@ -4602,19 +5805,19 @@
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
       <c r="I10" s="38"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="67"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="59"/>
       <c r="L10" s="36"/>
       <c r="M10" s="37"/>
       <c r="N10" s="37"/>
       <c r="O10" s="37"/>
       <c r="P10" s="38"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="57"/>
-      <c r="T10" s="57"/>
-      <c r="U10" s="57"/>
-      <c r="V10" s="58"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="64"/>
       <c r="W10" s="17"/>
       <c r="X10" s="18"/>
       <c r="Y10" s="18"/>
@@ -4630,21 +5833,21 @@
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
       <c r="I11" s="38"/>
-      <c r="J11" s="62" t="s">
+      <c r="J11" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="63"/>
+      <c r="K11" s="55"/>
       <c r="L11" s="36"/>
       <c r="M11" s="37"/>
       <c r="N11" s="37"/>
       <c r="O11" s="37"/>
       <c r="P11" s="38"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="57"/>
-      <c r="U11" s="57"/>
-      <c r="V11" s="58"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="64"/>
       <c r="W11" s="17"/>
       <c r="X11" s="18"/>
       <c r="Y11" s="18"/>
@@ -4660,19 +5863,19 @@
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="38"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="65"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="57"/>
       <c r="L12" s="36"/>
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
       <c r="O12" s="37"/>
       <c r="P12" s="38"/>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="57"/>
-      <c r="U12" s="57"/>
-      <c r="V12" s="58"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="64"/>
       <c r="W12" s="17"/>
       <c r="X12" s="18"/>
       <c r="Y12" s="18"/>
@@ -4688,19 +5891,19 @@
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="38"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="65"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="36"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
       <c r="O13" s="37"/>
       <c r="P13" s="38"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="57"/>
-      <c r="V13" s="58"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="64"/>
       <c r="W13" s="17"/>
       <c r="X13" s="18"/>
       <c r="Y13" s="18"/>
@@ -4716,19 +5919,19 @@
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="65"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="36"/>
       <c r="M14" s="37"/>
       <c r="N14" s="37"/>
       <c r="O14" s="37"/>
       <c r="P14" s="38"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="58"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="64"/>
       <c r="W14" s="17"/>
       <c r="X14" s="18"/>
       <c r="Y14" s="18"/>
@@ -4744,19 +5947,19 @@
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" s="41"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="67"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="59"/>
       <c r="L15" s="39"/>
       <c r="M15" s="40"/>
       <c r="N15" s="40"/>
       <c r="O15" s="40"/>
       <c r="P15" s="41"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-      <c r="U15" s="60"/>
-      <c r="V15" s="61"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="67"/>
       <c r="W15" s="20"/>
       <c r="X15" s="21"/>
       <c r="Y15" s="21"/>
@@ -4868,7 +6071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z35"/>
   <sheetViews>
@@ -5018,10 +6221,10 @@
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
       <c r="I5" s="35"/>
-      <c r="J5" s="62" t="s">
+      <c r="J5" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="63"/>
+      <c r="K5" s="55"/>
       <c r="L5" s="33" t="s">
         <v>32</v>
       </c>
@@ -5054,8 +6257,8 @@
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
       <c r="I6" s="38"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="65"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
       <c r="L6" s="36"/>
       <c r="M6" s="37"/>
       <c r="N6" s="37"/>
@@ -5082,8 +6285,8 @@
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
       <c r="I7" s="38"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="65"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="36"/>
       <c r="M7" s="37"/>
       <c r="N7" s="37"/>
@@ -5110,8 +6313,8 @@
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
       <c r="I8" s="38"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="65"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
       <c r="L8" s="36"/>
       <c r="M8" s="37"/>
       <c r="N8" s="37"/>
@@ -5138,8 +6341,8 @@
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
       <c r="I9" s="38"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="65"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="36"/>
       <c r="M9" s="37"/>
       <c r="N9" s="37"/>
@@ -5166,8 +6369,8 @@
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
       <c r="I10" s="38"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="67"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="59"/>
       <c r="L10" s="36"/>
       <c r="M10" s="37"/>
       <c r="N10" s="37"/>
@@ -5194,10 +6397,10 @@
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
       <c r="I11" s="38"/>
-      <c r="J11" s="62" t="s">
+      <c r="J11" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="K11" s="63"/>
+      <c r="K11" s="55"/>
       <c r="L11" s="36"/>
       <c r="M11" s="37"/>
       <c r="N11" s="37"/>
@@ -5224,8 +6427,8 @@
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="38"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="65"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="57"/>
       <c r="L12" s="36"/>
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
@@ -5252,8 +6455,8 @@
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="38"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="65"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="36"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
@@ -5280,8 +6483,8 @@
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="65"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="36"/>
       <c r="M14" s="37"/>
       <c r="N14" s="37"/>
@@ -5308,8 +6511,8 @@
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" s="41"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="67"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="59"/>
       <c r="L15" s="39"/>
       <c r="M15" s="40"/>
       <c r="N15" s="40"/>
@@ -5433,7 +6636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z35"/>
   <sheetViews>
@@ -5583,10 +6786,10 @@
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
       <c r="I5" s="35"/>
-      <c r="J5" s="62" t="s">
+      <c r="J5" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="63"/>
+      <c r="K5" s="55"/>
       <c r="L5" s="33" t="s">
         <v>61</v>
       </c>
@@ -5597,11 +6800,11 @@
       <c r="Q5" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
-      <c r="V5" s="55"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="61"/>
       <c r="W5" s="31" t="s">
         <v>8</v>
       </c>
@@ -5619,19 +6822,19 @@
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
       <c r="I6" s="38"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="65"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
       <c r="L6" s="36"/>
       <c r="M6" s="37"/>
       <c r="N6" s="37"/>
       <c r="O6" s="37"/>
       <c r="P6" s="37"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="57"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="57"/>
-      <c r="U6" s="57"/>
-      <c r="V6" s="58"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="64"/>
       <c r="W6" s="17"/>
       <c r="X6" s="18"/>
       <c r="Y6" s="18"/>
@@ -5647,19 +6850,19 @@
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
       <c r="I7" s="38"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="65"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="36"/>
       <c r="M7" s="37"/>
       <c r="N7" s="37"/>
       <c r="O7" s="37"/>
       <c r="P7" s="37"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="57"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="57"/>
-      <c r="V7" s="58"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="64"/>
       <c r="W7" s="17"/>
       <c r="X7" s="18"/>
       <c r="Y7" s="18"/>
@@ -5675,19 +6878,19 @@
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
       <c r="I8" s="38"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="65"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
       <c r="L8" s="36"/>
       <c r="M8" s="37"/>
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
       <c r="P8" s="37"/>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="57"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="57"/>
-      <c r="U8" s="57"/>
-      <c r="V8" s="58"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="64"/>
       <c r="W8" s="17"/>
       <c r="X8" s="18"/>
       <c r="Y8" s="18"/>
@@ -5703,19 +6906,19 @@
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
       <c r="I9" s="38"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="65"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="36"/>
       <c r="M9" s="37"/>
       <c r="N9" s="37"/>
       <c r="O9" s="37"/>
       <c r="P9" s="37"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
-      <c r="U9" s="57"/>
-      <c r="V9" s="58"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="64"/>
       <c r="W9" s="17"/>
       <c r="X9" s="18"/>
       <c r="Y9" s="18"/>
@@ -5731,19 +6934,19 @@
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
       <c r="I10" s="38"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="67"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="59"/>
       <c r="L10" s="36"/>
       <c r="M10" s="37"/>
       <c r="N10" s="37"/>
       <c r="O10" s="37"/>
       <c r="P10" s="37"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="57"/>
-      <c r="T10" s="57"/>
-      <c r="U10" s="57"/>
-      <c r="V10" s="58"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="64"/>
       <c r="W10" s="17"/>
       <c r="X10" s="18"/>
       <c r="Y10" s="18"/>
@@ -5759,21 +6962,21 @@
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
       <c r="I11" s="38"/>
-      <c r="J11" s="62" t="s">
+      <c r="J11" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="63"/>
+      <c r="K11" s="55"/>
       <c r="L11" s="36"/>
       <c r="M11" s="37"/>
       <c r="N11" s="37"/>
       <c r="O11" s="37"/>
       <c r="P11" s="37"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="57"/>
-      <c r="U11" s="57"/>
-      <c r="V11" s="58"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="64"/>
       <c r="W11" s="17"/>
       <c r="X11" s="18"/>
       <c r="Y11" s="18"/>
@@ -5789,19 +6992,19 @@
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="38"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="65"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="57"/>
       <c r="L12" s="36"/>
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
       <c r="O12" s="37"/>
       <c r="P12" s="37"/>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="57"/>
-      <c r="U12" s="57"/>
-      <c r="V12" s="58"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="64"/>
       <c r="W12" s="17"/>
       <c r="X12" s="18"/>
       <c r="Y12" s="18"/>
@@ -5817,19 +7020,19 @@
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="38"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="65"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="36"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
       <c r="O13" s="37"/>
       <c r="P13" s="37"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="57"/>
-      <c r="V13" s="58"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="64"/>
       <c r="W13" s="17"/>
       <c r="X13" s="18"/>
       <c r="Y13" s="18"/>
@@ -5845,19 +7048,19 @@
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="65"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="36"/>
       <c r="M14" s="37"/>
       <c r="N14" s="37"/>
       <c r="O14" s="37"/>
       <c r="P14" s="37"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="58"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="64"/>
       <c r="W14" s="17"/>
       <c r="X14" s="18"/>
       <c r="Y14" s="18"/>
@@ -5873,19 +7076,19 @@
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" s="41"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="67"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="59"/>
       <c r="L15" s="39"/>
       <c r="M15" s="40"/>
       <c r="N15" s="40"/>
       <c r="O15" s="40"/>
       <c r="P15" s="40"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-      <c r="U15" s="60"/>
-      <c r="V15" s="61"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="67"/>
       <c r="W15" s="20"/>
       <c r="X15" s="21"/>
       <c r="Y15" s="21"/>
@@ -5998,12 +7201,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5:V15"/>
+      <selection activeCell="J5" sqref="J5:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6162,11 +7365,11 @@
       <c r="Q5" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
-      <c r="V5" s="55"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="61"/>
       <c r="W5" s="31" t="s">
         <v>8</v>
       </c>
@@ -6191,12 +7394,12 @@
       <c r="N6" s="37"/>
       <c r="O6" s="37"/>
       <c r="P6" s="37"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="57"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="57"/>
-      <c r="U6" s="57"/>
-      <c r="V6" s="58"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="64"/>
       <c r="W6" s="17"/>
       <c r="X6" s="18"/>
       <c r="Y6" s="18"/>
@@ -6219,12 +7422,12 @@
       <c r="N7" s="37"/>
       <c r="O7" s="37"/>
       <c r="P7" s="37"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="57"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="57"/>
-      <c r="V7" s="58"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="64"/>
       <c r="W7" s="17"/>
       <c r="X7" s="18"/>
       <c r="Y7" s="18"/>
@@ -6247,12 +7450,12 @@
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
       <c r="P8" s="37"/>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="57"/>
-      <c r="S8" s="57"/>
-      <c r="T8" s="57"/>
-      <c r="U8" s="57"/>
-      <c r="V8" s="58"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="64"/>
       <c r="W8" s="17"/>
       <c r="X8" s="18"/>
       <c r="Y8" s="18"/>
@@ -6275,12 +7478,12 @@
       <c r="N9" s="37"/>
       <c r="O9" s="37"/>
       <c r="P9" s="37"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
-      <c r="U9" s="57"/>
-      <c r="V9" s="58"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="64"/>
       <c r="W9" s="17"/>
       <c r="X9" s="18"/>
       <c r="Y9" s="18"/>
@@ -6303,12 +7506,12 @@
       <c r="N10" s="37"/>
       <c r="O10" s="37"/>
       <c r="P10" s="37"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="57"/>
-      <c r="T10" s="57"/>
-      <c r="U10" s="57"/>
-      <c r="V10" s="58"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="64"/>
       <c r="W10" s="17"/>
       <c r="X10" s="18"/>
       <c r="Y10" s="18"/>
@@ -6327,18 +7530,18 @@
       <c r="J11" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="76"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="36"/>
       <c r="M11" s="37"/>
       <c r="N11" s="37"/>
       <c r="O11" s="37"/>
       <c r="P11" s="37"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="57"/>
-      <c r="U11" s="57"/>
-      <c r="V11" s="58"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="64"/>
       <c r="W11" s="17"/>
       <c r="X11" s="18"/>
       <c r="Y11" s="18"/>
@@ -6354,19 +7557,19 @@
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="38"/>
-      <c r="J12" s="77"/>
-      <c r="K12" s="78"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="71"/>
       <c r="L12" s="36"/>
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
       <c r="O12" s="37"/>
       <c r="P12" s="37"/>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="57"/>
-      <c r="U12" s="57"/>
-      <c r="V12" s="58"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="64"/>
       <c r="W12" s="17"/>
       <c r="X12" s="18"/>
       <c r="Y12" s="18"/>
@@ -6382,19 +7585,19 @@
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="38"/>
-      <c r="J13" s="77"/>
-      <c r="K13" s="78"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="71"/>
       <c r="L13" s="36"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
       <c r="O13" s="37"/>
       <c r="P13" s="37"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="57"/>
-      <c r="V13" s="58"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="64"/>
       <c r="W13" s="17"/>
       <c r="X13" s="18"/>
       <c r="Y13" s="18"/>
@@ -6410,19 +7613,19 @@
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="78"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="71"/>
       <c r="L14" s="36"/>
       <c r="M14" s="37"/>
       <c r="N14" s="37"/>
       <c r="O14" s="37"/>
       <c r="P14" s="37"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="58"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="64"/>
       <c r="W14" s="17"/>
       <c r="X14" s="18"/>
       <c r="Y14" s="18"/>
@@ -6438,19 +7641,19 @@
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" s="41"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="80"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="73"/>
       <c r="L15" s="39"/>
       <c r="M15" s="40"/>
       <c r="N15" s="40"/>
       <c r="O15" s="40"/>
       <c r="P15" s="40"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-      <c r="U15" s="60"/>
-      <c r="V15" s="61"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="67"/>
       <c r="W15" s="20"/>
       <c r="X15" s="21"/>
       <c r="Y15" s="21"/>
@@ -6561,566 +7764,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z35"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5:Z15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A1" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="12"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="19"/>
-    </row>
-    <row r="3" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="20"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="22"/>
-    </row>
-    <row r="4" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="22"/>
-    </row>
-    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="K5" s="69"/>
-      <c r="L5" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="12"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A6" s="27"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="38"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="19"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A7" s="27"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="38"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="19"/>
-    </row>
-    <row r="8" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="37"/>
-      <c r="V8" s="38"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="18"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="19"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A9" s="27"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
-      <c r="V9" s="38"/>
-      <c r="W9" s="17"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="19"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="37"/>
-      <c r="N10" s="37"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="37"/>
-      <c r="U10" s="37"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="19"/>
-    </row>
-    <row r="11" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="27"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="70"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="37"/>
-      <c r="U11" s="37"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="19"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A12" s="27"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="37"/>
-      <c r="S12" s="37"/>
-      <c r="T12" s="37"/>
-      <c r="U12" s="37"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="17"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="19"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A13" s="27"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
-      <c r="U13" s="37"/>
-      <c r="V13" s="38"/>
-      <c r="W13" s="17"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="19"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A14" s="27"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="71"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="37"/>
-      <c r="V14" s="38"/>
-      <c r="W14" s="17"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="19"/>
-    </row>
-    <row r="15" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="29"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="73"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="40"/>
-      <c r="S15" s="40"/>
-      <c r="T15" s="40"/>
-      <c r="U15" s="40"/>
-      <c r="V15" s="41"/>
-      <c r="W15" s="20"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="22"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A5:B15"/>
-    <mergeCell ref="C5:I15"/>
-    <mergeCell ref="L5:P15"/>
-    <mergeCell ref="Q5:V15"/>
-    <mergeCell ref="W5:Z15"/>
-    <mergeCell ref="J5:K15"/>
-    <mergeCell ref="A1:Z3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:P4"/>
-    <mergeCell ref="Q4:V4"/>
-    <mergeCell ref="W4:Z4"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="J5:K15" r:id="rId1" display="https://github.com/phc09188/JSP-Study/tree/main/src/main/webapp"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
chapter 13 custom tag 02.14 내일 다시해야함
</commit_message>
<xml_diff>
--- a/JSP-SERVLET.xlsx
+++ b/JSP-SERVLET.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="12"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="현황" sheetId="9" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <sheet name="Chapter 9" sheetId="12" r:id="rId11"/>
     <sheet name="Chapter 10" sheetId="13" r:id="rId12"/>
     <sheet name="Chapter 11" sheetId="15" r:id="rId13"/>
+    <sheet name="Chapter 12" sheetId="16" r:id="rId14"/>
+    <sheet name="Chapter 13" sheetId="17" r:id="rId15"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="94">
   <si>
     <t>페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -523,6 +525,25 @@
   <si>
     <t xml:space="preserve">JSP
 dataSource,jdbc.jsp
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">P.415 ~ P.430
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. EL(Expression Language)란?
+2. EL 표현식 
+3. EL 내장객체 사용 및 실습 
+4. header, session application 정보 추출
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">JSP
+(bookInput,bookOutput,bookprocess.jsp)
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1523,6 +1544,25 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C17:D17"/>
@@ -1537,25 +1577,6 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2100,6 +2121,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="C5:I15"/>
+    <mergeCell ref="L5:P15"/>
+    <mergeCell ref="Q5:V15"/>
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="J5:K15"/>
     <mergeCell ref="A1:Z3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:I4"/>
@@ -2107,12 +2134,6 @@
     <mergeCell ref="L4:P4"/>
     <mergeCell ref="Q4:V4"/>
     <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="A5:B15"/>
-    <mergeCell ref="C5:I15"/>
-    <mergeCell ref="L5:P15"/>
-    <mergeCell ref="Q5:V15"/>
-    <mergeCell ref="W5:Z15"/>
-    <mergeCell ref="J5:K15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2690,7 +2711,7 @@
   <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="J5" sqref="J5:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3254,7 +3275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -3788,12 +3809,576 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:Z3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="W4:Z4"/>
     <mergeCell ref="A5:B15"/>
     <mergeCell ref="C5:I15"/>
     <mergeCell ref="L5:P15"/>
     <mergeCell ref="Q5:V15"/>
     <mergeCell ref="W5:Z15"/>
     <mergeCell ref="J5:K15"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J5:K15" r:id="rId1" display="https://github.com/phc09188/JSP-Study/tree/main/src/main/webapp"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z35"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="12"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="19"/>
+    </row>
+    <row r="3" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="22"/>
+    </row>
+    <row r="4" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="24"/>
+      <c r="L4" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="22"/>
+    </row>
+    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="75"/>
+      <c r="L5" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="61"/>
+      <c r="W5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="12"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="19"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="64"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="19"/>
+    </row>
+    <row r="8" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="64"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="19"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="19"/>
+    </row>
+    <row r="10" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="64"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="19"/>
+    </row>
+    <row r="11" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="69"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="19"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="64"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="19"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A13" s="27"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="64"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="19"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="64"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="19"/>
+    </row>
+    <row r="15" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="67"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
+      <c r="Z15" s="22"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="C5:I15"/>
+    <mergeCell ref="L5:P15"/>
+    <mergeCell ref="Q5:V15"/>
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="J5:K10"/>
+    <mergeCell ref="J11:K15"/>
     <mergeCell ref="A1:Z3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:I4"/>
@@ -3804,10 +4389,578 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J5:K15" r:id="rId1" display="https://github.com/phc09188/JSP-Study/tree/main/src/main/webapp"/>
+    <hyperlink ref="J11:K15" r:id="rId1" display="https://github.com/phc09188/JSP-Study/blob/main/src/main/java/com/example/jsptest/chapter10/beans/HelloBean.java"/>
+    <hyperlink ref="J5:K10" r:id="rId2" display="https://github.com/phc09188/JSP-Study/blob/main/src/main/webapp/been.jsp"/>
+    <hyperlink ref="J5:K15" r:id="rId3" display="https://github.com/phc09188/JSP-Study/blob/main/src/main/java/com/example/jsptest/chapter12/BookBean.java"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="12"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="19"/>
+    </row>
+    <row r="3" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="22"/>
+    </row>
+    <row r="4" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="24"/>
+      <c r="L4" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="22"/>
+    </row>
+    <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="75"/>
+      <c r="L5" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="61"/>
+      <c r="W5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="12"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="19"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="64"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="19"/>
+    </row>
+    <row r="8" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="64"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="19"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="19"/>
+    </row>
+    <row r="10" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="64"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="19"/>
+    </row>
+    <row r="11" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="69"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="19"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
+      <c r="V12" s="64"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="19"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A13" s="27"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="63"/>
+      <c r="V13" s="64"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="19"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="64"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="19"/>
+    </row>
+    <row r="15" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="65"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="67"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
+      <c r="Z15" s="22"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="C5:I15"/>
+    <mergeCell ref="J5:K10"/>
+    <mergeCell ref="L5:P15"/>
+    <mergeCell ref="Q5:V15"/>
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="J11:K15"/>
+    <mergeCell ref="A1:Z3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="W4:Z4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J11:K15" r:id="rId1" display="https://github.com/phc09188/JSP-Study/blob/main/src/main/java/com/example/jsptest/chapter10/beans/HelloBean.java"/>
+    <hyperlink ref="J5:K10" r:id="rId2" display="https://github.com/phc09188/JSP-Study/blob/main/src/main/webapp/been.jsp"/>
+    <hyperlink ref="J5:K15" r:id="rId3" display="https://github.com/phc09188/JSP-Study/blob/main/src/main/java/com/example/jsptest/chapter12/BookBean.java"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -4921,12 +6074,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A5:B15"/>
-    <mergeCell ref="O5:R15"/>
-    <mergeCell ref="S5:V15"/>
-    <mergeCell ref="W5:Z15"/>
-    <mergeCell ref="J5:N15"/>
-    <mergeCell ref="C5:I15"/>
     <mergeCell ref="A1:Z3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="O4:R4"/>
@@ -4934,6 +6081,12 @@
     <mergeCell ref="W4:Z4"/>
     <mergeCell ref="J4:N4"/>
     <mergeCell ref="C4:I4"/>
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="O5:R15"/>
+    <mergeCell ref="S5:V15"/>
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="J5:N15"/>
+    <mergeCell ref="C5:I15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
chapter 13 custom tag 마무리
</commit_message>
<xml_diff>
--- a/JSP-SERVLET.xlsx
+++ b/JSP-SERVLET.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="100">
   <si>
     <t>페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -545,6 +545,39 @@
     <t xml:space="preserve">JSP
 (bookInput,bookOutput,bookprocess.jsp)
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">P.431 ~ P.485
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 클래스 기반 커스텀 태그 실습
+(jsp1.2 방식 &amp; jsp2.0방식)
+2. 태그 기반 커스텀 태그 실습
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 커스텀 태그란?
+2. 클래스 기반 커스텀 태그 설명 및 실습
+3. 태그 기반 커스텀태그(jsp 파일의 확장자를 tag로 사용)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Tag
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">클래스 기반 Tag
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커스텀 태그</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1544,25 +1577,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C17:D17"/>
@@ -1577,6 +1591,25 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2121,12 +2154,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A5:B15"/>
-    <mergeCell ref="C5:I15"/>
-    <mergeCell ref="L5:P15"/>
-    <mergeCell ref="Q5:V15"/>
-    <mergeCell ref="W5:Z15"/>
-    <mergeCell ref="J5:K15"/>
     <mergeCell ref="A1:Z3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:I4"/>
@@ -2134,6 +2161,12 @@
     <mergeCell ref="L4:P4"/>
     <mergeCell ref="Q4:V4"/>
     <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="C5:I15"/>
+    <mergeCell ref="L5:P15"/>
+    <mergeCell ref="Q5:V15"/>
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="J5:K15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3809,6 +3842,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="C5:I15"/>
+    <mergeCell ref="L5:P15"/>
+    <mergeCell ref="Q5:V15"/>
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="J5:K15"/>
     <mergeCell ref="A1:Z3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:I4"/>
@@ -3816,12 +3855,6 @@
     <mergeCell ref="L4:P4"/>
     <mergeCell ref="Q4:V4"/>
     <mergeCell ref="W4:Z4"/>
-    <mergeCell ref="A5:B15"/>
-    <mergeCell ref="C5:I15"/>
-    <mergeCell ref="L5:P15"/>
-    <mergeCell ref="Q5:V15"/>
-    <mergeCell ref="W5:Z15"/>
-    <mergeCell ref="J5:K15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -4372,6 +4405,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:Z3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="Q4:V4"/>
+    <mergeCell ref="W4:Z4"/>
     <mergeCell ref="A5:B15"/>
     <mergeCell ref="C5:I15"/>
     <mergeCell ref="L5:P15"/>
@@ -4379,13 +4419,6 @@
     <mergeCell ref="W5:Z15"/>
     <mergeCell ref="J5:K10"/>
     <mergeCell ref="J11:K15"/>
-    <mergeCell ref="A1:Z3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:P4"/>
-    <mergeCell ref="Q4:V4"/>
-    <mergeCell ref="W4:Z4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -4403,14 +4436,14 @@
   <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4536,11 +4569,11 @@
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="33" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
@@ -4548,12 +4581,12 @@
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
       <c r="I5" s="35"/>
-      <c r="J5" s="74" t="s">
+      <c r="J5" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="K5" s="75"/>
+      <c r="K5" s="76"/>
       <c r="L5" s="33" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="M5" s="34"/>
       <c r="N5" s="34"/>
@@ -4584,8 +4617,8 @@
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
       <c r="I6" s="38"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="78"/>
       <c r="L6" s="36"/>
       <c r="M6" s="37"/>
       <c r="N6" s="37"/>
@@ -4612,8 +4645,8 @@
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
       <c r="I7" s="38"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="78"/>
       <c r="L7" s="36"/>
       <c r="M7" s="37"/>
       <c r="N7" s="37"/>
@@ -4630,7 +4663,7 @@
       <c r="Y7" s="18"/>
       <c r="Z7" s="19"/>
     </row>
-    <row r="8" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="27"/>
       <c r="B8" s="28"/>
       <c r="C8" s="36"/>
@@ -4640,8 +4673,8 @@
       <c r="G8" s="37"/>
       <c r="H8" s="37"/>
       <c r="I8" s="38"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="80"/>
       <c r="L8" s="36"/>
       <c r="M8" s="37"/>
       <c r="N8" s="37"/>
@@ -4658,7 +4691,7 @@
       <c r="Y8" s="18"/>
       <c r="Z8" s="19"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="27"/>
       <c r="B9" s="28"/>
       <c r="C9" s="36"/>
@@ -4668,8 +4701,10 @@
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
       <c r="I9" s="38"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
+      <c r="J9" s="77" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" s="78"/>
       <c r="L9" s="36"/>
       <c r="M9" s="37"/>
       <c r="N9" s="37"/>
@@ -4686,7 +4721,7 @@
       <c r="Y9" s="18"/>
       <c r="Z9" s="19"/>
     </row>
-    <row r="10" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A10" s="27"/>
       <c r="B10" s="28"/>
       <c r="C10" s="36"/>
@@ -4696,8 +4731,8 @@
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
       <c r="I10" s="38"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="78"/>
       <c r="L10" s="36"/>
       <c r="M10" s="37"/>
       <c r="N10" s="37"/>
@@ -4724,10 +4759,8 @@
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
       <c r="I11" s="38"/>
-      <c r="J11" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" s="69"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="78"/>
       <c r="L11" s="36"/>
       <c r="M11" s="37"/>
       <c r="N11" s="37"/>
@@ -4744,7 +4777,7 @@
       <c r="Y11" s="18"/>
       <c r="Z11" s="19"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="27"/>
       <c r="B12" s="28"/>
       <c r="C12" s="36"/>
@@ -4754,8 +4787,8 @@
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="38"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="71"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="78"/>
       <c r="L12" s="36"/>
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
@@ -4782,8 +4815,10 @@
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="38"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="71"/>
+      <c r="J13" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" s="76"/>
       <c r="L13" s="36"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
@@ -4810,8 +4845,8 @@
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="71"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="78"/>
       <c r="L14" s="36"/>
       <c r="M14" s="37"/>
       <c r="N14" s="37"/>
@@ -4838,8 +4873,8 @@
       <c r="G15" s="40"/>
       <c r="H15" s="40"/>
       <c r="I15" s="41"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="73"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="80"/>
       <c r="L15" s="39"/>
       <c r="M15" s="40"/>
       <c r="N15" s="40"/>
@@ -4937,14 +4972,8 @@
       <c r="B35" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A5:B15"/>
-    <mergeCell ref="C5:I15"/>
-    <mergeCell ref="J5:K10"/>
-    <mergeCell ref="L5:P15"/>
-    <mergeCell ref="Q5:V15"/>
+  <mergeCells count="15">
     <mergeCell ref="W5:Z15"/>
-    <mergeCell ref="J11:K15"/>
     <mergeCell ref="A1:Z3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:I4"/>
@@ -4952,15 +4981,17 @@
     <mergeCell ref="L4:P4"/>
     <mergeCell ref="Q4:V4"/>
     <mergeCell ref="W4:Z4"/>
+    <mergeCell ref="J5:K8"/>
+    <mergeCell ref="J9:K12"/>
+    <mergeCell ref="J13:K15"/>
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="C5:I15"/>
+    <mergeCell ref="L5:P15"/>
+    <mergeCell ref="Q5:V15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="J11:K15" r:id="rId1" display="https://github.com/phc09188/JSP-Study/blob/main/src/main/java/com/example/jsptest/chapter10/beans/HelloBean.java"/>
-    <hyperlink ref="J5:K10" r:id="rId2" display="https://github.com/phc09188/JSP-Study/blob/main/src/main/webapp/been.jsp"/>
-    <hyperlink ref="J5:K15" r:id="rId3" display="https://github.com/phc09188/JSP-Study/blob/main/src/main/java/com/example/jsptest/chapter12/BookBean.java"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6074,6 +6105,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A5:B15"/>
+    <mergeCell ref="O5:R15"/>
+    <mergeCell ref="S5:V15"/>
+    <mergeCell ref="W5:Z15"/>
+    <mergeCell ref="J5:N15"/>
+    <mergeCell ref="C5:I15"/>
     <mergeCell ref="A1:Z3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="O4:R4"/>
@@ -6081,12 +6118,6 @@
     <mergeCell ref="W4:Z4"/>
     <mergeCell ref="J4:N4"/>
     <mergeCell ref="C4:I4"/>
-    <mergeCell ref="A5:B15"/>
-    <mergeCell ref="O5:R15"/>
-    <mergeCell ref="S5:V15"/>
-    <mergeCell ref="W5:Z15"/>
-    <mergeCell ref="J5:N15"/>
-    <mergeCell ref="C5:I15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>